<commit_message>
update fix - 1
</commit_message>
<xml_diff>
--- a/Master_Driver.xlsx
+++ b/Master_Driver.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Documents\@Afi\@MileApp Data\@Program GUI\Truck_Usage\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Documents\@Afi\@TMS Data\@Program GUI\@GUI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51758DC1-706D-405A-B333-3B585EF76381}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD83D64A-80E7-40F8-A708-4FF6EF77BC3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="18810" windowHeight="11295" xr2:uid="{91B95C4E-923A-41B3-81DC-B922A7F05DB7}"/>
+    <workbookView xWindow="3720" yWindow="3720" windowWidth="18810" windowHeight="11295" xr2:uid="{91B95C4E-923A-41B3-81DC-B922A7F05DB7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -354,9 +354,6 @@
     <t>W 9335 PG</t>
   </si>
   <si>
-    <t>W 9731 NX</t>
-  </si>
-  <si>
     <t>W 9971 PF</t>
   </si>
   <si>
@@ -439,6 +436,9 @@
   </si>
   <si>
     <t>DRY-CDE-LONG-2500</t>
+  </si>
+  <si>
+    <t>W 8059 QH</t>
   </si>
 </sst>
 </file>
@@ -877,8 +877,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE67EB79-B615-476E-BCC8-C5C1A719DDF9}">
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -898,10 +898,10 @@
         <v>52</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -915,7 +915,7 @@
         <v>79</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -929,7 +929,7 @@
         <v>80</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -943,7 +943,7 @@
         <v>81</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -957,7 +957,7 @@
         <v>82</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -965,13 +965,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>83</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -979,13 +979,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>84</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -993,13 +993,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>85</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1013,7 +1013,7 @@
         <v>86</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1027,7 +1027,7 @@
         <v>87</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1041,7 +1041,7 @@
         <v>88</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1055,7 +1055,7 @@
         <v>89</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1069,7 +1069,7 @@
         <v>90</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1083,7 +1083,7 @@
         <v>91</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1091,13 +1091,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>92</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1111,7 +1111,7 @@
         <v>93</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1119,13 +1119,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>94</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1139,7 +1139,7 @@
         <v>95</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1147,13 +1147,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>96</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1161,13 +1161,13 @@
         <v>19</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>97</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1181,7 +1181,7 @@
         <v>98</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1195,7 +1195,7 @@
         <v>99</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1209,7 +1209,7 @@
         <v>100</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1223,7 +1223,7 @@
         <v>101</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1231,13 +1231,13 @@
         <v>24</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>102</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1251,7 +1251,7 @@
         <v>103</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1259,13 +1259,13 @@
         <v>26</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>104</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1279,7 +1279,7 @@
         <v>105</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1290,10 +1290,10 @@
         <v>49</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>106</v>
+        <v>134</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1304,10 +1304,10 @@
         <v>50</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1318,10 +1318,10 @@
         <v>51</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1335,7 +1335,7 @@
         <v>69</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1349,7 +1349,7 @@
         <v>70</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1357,13 +1357,13 @@
         <v>55</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>71</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1371,13 +1371,13 @@
         <v>56</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>72</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1391,7 +1391,7 @@
         <v>73</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1405,7 +1405,7 @@
         <v>74</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1419,7 +1419,7 @@
         <v>75</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1427,13 +1427,13 @@
         <v>60</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>76</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1447,7 +1447,7 @@
         <v>77</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1455,13 +1455,13 @@
         <v>62</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>78</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change processing excel file
</commit_message>
<xml_diff>
--- a/Master_Driver.xlsx
+++ b/Master_Driver.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Documents\@Afi\@MileApp Data\@Program GUI\Truck_Usage\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Documents\@Afi\@TMS Data\@Program GUI\@GUI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51758DC1-706D-405A-B333-3B585EF76381}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD83D64A-80E7-40F8-A708-4FF6EF77BC3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="18810" windowHeight="11295" xr2:uid="{91B95C4E-923A-41B3-81DC-B922A7F05DB7}"/>
+    <workbookView xWindow="3720" yWindow="3720" windowWidth="18810" windowHeight="11295" xr2:uid="{91B95C4E-923A-41B3-81DC-B922A7F05DB7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -354,9 +354,6 @@
     <t>W 9335 PG</t>
   </si>
   <si>
-    <t>W 9731 NX</t>
-  </si>
-  <si>
     <t>W 9971 PF</t>
   </si>
   <si>
@@ -439,6 +436,9 @@
   </si>
   <si>
     <t>DRY-CDE-LONG-2500</t>
+  </si>
+  <si>
+    <t>W 8059 QH</t>
   </si>
 </sst>
 </file>
@@ -877,8 +877,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE67EB79-B615-476E-BCC8-C5C1A719DDF9}">
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -898,10 +898,10 @@
         <v>52</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -915,7 +915,7 @@
         <v>79</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -929,7 +929,7 @@
         <v>80</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -943,7 +943,7 @@
         <v>81</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -957,7 +957,7 @@
         <v>82</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -965,13 +965,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>83</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -979,13 +979,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>84</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -993,13 +993,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>85</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1013,7 +1013,7 @@
         <v>86</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1027,7 +1027,7 @@
         <v>87</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1041,7 +1041,7 @@
         <v>88</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1055,7 +1055,7 @@
         <v>89</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1069,7 +1069,7 @@
         <v>90</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1083,7 +1083,7 @@
         <v>91</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1091,13 +1091,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>92</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1111,7 +1111,7 @@
         <v>93</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1119,13 +1119,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>94</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1139,7 +1139,7 @@
         <v>95</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1147,13 +1147,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>96</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1161,13 +1161,13 @@
         <v>19</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>97</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1181,7 +1181,7 @@
         <v>98</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1195,7 +1195,7 @@
         <v>99</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1209,7 +1209,7 @@
         <v>100</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1223,7 +1223,7 @@
         <v>101</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1231,13 +1231,13 @@
         <v>24</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>102</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1251,7 +1251,7 @@
         <v>103</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1259,13 +1259,13 @@
         <v>26</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>104</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1279,7 +1279,7 @@
         <v>105</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1290,10 +1290,10 @@
         <v>49</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>106</v>
+        <v>134</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1304,10 +1304,10 @@
         <v>50</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1318,10 +1318,10 @@
         <v>51</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1335,7 +1335,7 @@
         <v>69</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1349,7 +1349,7 @@
         <v>70</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1357,13 +1357,13 @@
         <v>55</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>71</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1371,13 +1371,13 @@
         <v>56</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>72</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1391,7 +1391,7 @@
         <v>73</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1405,7 +1405,7 @@
         <v>74</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1419,7 +1419,7 @@
         <v>75</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1427,13 +1427,13 @@
         <v>60</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>76</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1447,7 +1447,7 @@
         <v>77</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1455,13 +1455,13 @@
         <v>62</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>78</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>